<commit_message>
commit functional xlsx generation code
</commit_message>
<xml_diff>
--- a/assets/generated/model2/ArrivalAtCustomerTime.xlsx
+++ b/assets/generated/model2/ArrivalAtCustomerTime.xlsx
@@ -340,12 +340,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3">
+        <v>27.00000000000221</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8">
+        <v>30.00000000001455</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
commit model 2 results, model needs debugging
</commit_message>
<xml_diff>
--- a/assets/generated/model2/ArrivalAtCustomerTime.xlsx
+++ b/assets/generated/model2/ArrivalAtCustomerTime.xlsx
@@ -348,42 +348,42 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1">
-        <v>97</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2">
-        <v>27</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3">
-        <v>27.00000000000221</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4">
-        <v>27</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5">
-        <v>27</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6">
-        <v>19</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7">
-        <v>20</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8">
-        <v>30.00000000001455</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
functional model need to fix variables
</commit_message>
<xml_diff>
--- a/assets/generated/model2/ArrivalAtCustomerTime.xlsx
+++ b/assets/generated/model2/ArrivalAtCustomerTime.xlsx
@@ -348,42 +348,42 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1">
-        <v>174</v>
+        <v>6541</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2">
-        <v>50</v>
+        <v>6544</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3">
-        <v>116</v>
+        <v>6547.999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4">
-        <v>149</v>
+        <v>6551</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5">
-        <v>34</v>
+        <v>6545.999959704648</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6">
-        <v>99</v>
+        <v>6537</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7">
-        <v>81</v>
+        <v>6547</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8">
-        <v>150</v>
+        <v>6551.999999999952</v>
       </c>
     </row>
   </sheetData>

</xml_diff>